<commit_message>
Fixed q1 concurrency issue
Same as q2 inaccurate counts: use synchronized instead of volatile you fool
</commit_message>
<xml_diff>
--- a/stack_performance.xlsx
+++ b/stack_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonycui/Documents/McGill/Semester 7/COMP 409/A3/Lock-free-Stack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A049957D-66C5-844B-BFF1-93CD34968558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67678082-9F28-734F-BF5C-ADBE949E6441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19400" yWindow="11920" windowWidth="13300" windowHeight="9660" xr2:uid="{7144C0E6-69BA-D64A-9EA4-93EFC50E4C43}"/>
+    <workbookView xWindow="-19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{7144C0E6-69BA-D64A-9EA4-93EFC50E4C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -59,13 +59,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,13 +89,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,7 +414,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <v>6747</v>
+        <v>6661</v>
       </c>
       <c r="H7">
         <v>6640</v>
@@ -574,12 +589,6 @@
       </c>
       <c r="F8">
         <v>6</v>
-      </c>
-      <c r="G8">
-        <v>6661</v>
-      </c>
-      <c r="I8">
-        <v>6936</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -619,7 +628,7 @@
         <f>AVERAGE(B3:B12)</f>
         <v>6718.4</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f t="shared" ref="C13:D13" si="0">AVERAGE(C3:C12)</f>
         <v>6674</v>
       </c>
@@ -627,9 +636,9 @@
         <f t="shared" si="0"/>
         <v>6683.8</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <f>AVERAGE(G3:G12)</f>
-        <v>6676.5</v>
+        <v>6662.4</v>
       </c>
       <c r="H13">
         <f t="shared" ref="H13" si="1">AVERAGE(H3:H12)</f>
@@ -637,7 +646,7 @@
       </c>
       <c r="I13">
         <f t="shared" ref="I13" si="2">AVERAGE(I3:I12)</f>
-        <v>6775.666666666667</v>
+        <v>6743.6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -712,7 +721,7 @@
         <v>6733</v>
       </c>
       <c r="D20">
-        <v>6639</v>
+        <v>6784</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -726,19 +735,13 @@
         <v>6823</v>
       </c>
       <c r="D21">
-        <v>6784</v>
+        <v>6796</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="C22">
-        <v>6928</v>
-      </c>
-      <c r="D22">
-        <v>6796</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -761,17 +764,17 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27">
+      <c r="B27" s="1">
         <f>AVERAGE(B17:B26)</f>
         <v>6606.8</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27:D27" si="3">AVERAGE(C17:C26)</f>
-        <v>6801.666666666667</v>
+        <v>6776.4</v>
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
-        <v>6763</v>
+        <v>6787.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>